<commit_message>
modifica per nuova richiesta accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ASCOM000000/ASCOM UMS/DIGISTAT/8/report-checklist.xlsx
+++ b/GATEWAY/S1#111ASCOM000000/ASCOM UMS/DIGISTAT/8/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itladi\Documents\My Notes\FSE\Accreditamento\Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541F03C5-069C-487C-B030-4ACFA2B2E0AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246D3AC4-F204-4DB3-9478-361979BC15BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="236">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -856,48 +856,9 @@
     <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.1e53fe6b3d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-04-07T09:32:44Z</t>
-  </si>
-  <si>
-    <t>c8de4d48a0496ad9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.e1c2e58aa8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-07T09:35:42Z</t>
-  </si>
-  <si>
-    <t>f075b34483e7ba57</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.04fe93e1f6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-07T09:37:15Z</t>
-  </si>
-  <si>
-    <t>373c3094b907cfa3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.f469b96f9e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-07T09:38:47Z</t>
-  </si>
-  <si>
-    <t>6f62736c9894a18a</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>2023-04-07T09:40:17Z</t>
-  </si>
-  <si>
-    <t>c32c34965d161976</t>
-  </si>
-  <si>
     <t>2023-04-07T09:42:31Z</t>
   </si>
   <si>
@@ -952,60 +913,6 @@
     <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.2b19d4c1ef^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-04-07T09:53:09Z</t>
-  </si>
-  <si>
-    <t>2d1f6041223f6d77</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.4e93edcb47^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-07T09:57:58Z</t>
-  </si>
-  <si>
-    <t>089d1e745df521dd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.7ac3eb5ef2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-07T09:59:16Z</t>
-  </si>
-  <si>
-    <t>43e274eb504dad28</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.38076fcbd5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-07T10:09:57Z</t>
-  </si>
-  <si>
-    <t>330becc94f4c12c7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.789aef2d7a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-07T10:11:22Z</t>
-  </si>
-  <si>
-    <t>10205a685cd554b2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.4cec0aebe4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-07T10:12:41Z</t>
-  </si>
-  <si>
-    <t>0f9f532336c3c3f2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.5510df097b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Viene segnalato un messaggio generico</t>
   </si>
   <si>
@@ -1082,6 +989,102 @@
   </si>
   <si>
     <t>Non applicabili in quanto pubblichiamo verso repository aziendale e non verso gateway regionale</t>
+  </si>
+  <si>
+    <t>2023-04-19T09:34:39Z</t>
+  </si>
+  <si>
+    <t>9d5d902aff7dda22</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.78f92ce44a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>19/4/2023</t>
+  </si>
+  <si>
+    <t>2023-04-19T09:39:02Z</t>
+  </si>
+  <si>
+    <t>bbb40be60b229bc8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.a9f84ca6a3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-19T09:40:48Z</t>
+  </si>
+  <si>
+    <t>9c94f3d06075072d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.b3730f6fde^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-19T09:49:42Z</t>
+  </si>
+  <si>
+    <t>efb861b36f0962be</t>
+  </si>
+  <si>
+    <t>2023-04-19T09:52:24Z</t>
+  </si>
+  <si>
+    <t>029ab58ce3047bfe</t>
+  </si>
+  <si>
+    <t>2023-04-19T10:14:31Z</t>
+  </si>
+  <si>
+    <t>54c7397131ec5eff</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.932792d1be^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-19T10:17:54Z</t>
+  </si>
+  <si>
+    <t>3274b3b6b4f47bf5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.cba00b8495^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-19T10:20:04Z</t>
+  </si>
+  <si>
+    <t>f17b964e63da0533</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.b61dddc10b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-19T10:22:11Z</t>
+  </si>
+  <si>
+    <t>ed087f975a46f8c4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.160235eca5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-19T10:25:06Z</t>
+  </si>
+  <si>
+    <t>5b29ca48736689cd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.8cbfc71966^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-19T10:27:14Z</t>
+  </si>
+  <si>
+    <t>96ff639528230eb0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.3.120915.4.4.32.11072433273.11.24aab23e81715b12cde8e57124f7bd6e9d3893e99899585f0a138148a086e1c7.aec04ddd7d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3995,10 +3998,10 @@
   <dimension ref="A1:T668"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4276,7 +4279,7 @@
         <v>151</v>
       </c>
       <c r="K10" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
@@ -4314,7 +4317,7 @@
         <v>151</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
@@ -4352,7 +4355,7 @@
         <v>151</v>
       </c>
       <c r="K12" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L12" s="25"/>
       <c r="M12" s="25"/>
@@ -4390,7 +4393,7 @@
         <v>151</v>
       </c>
       <c r="K13" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
@@ -4428,7 +4431,7 @@
         <v>151</v>
       </c>
       <c r="K14" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L14" s="25"/>
       <c r="M14" s="25"/>
@@ -4466,7 +4469,7 @@
         <v>151</v>
       </c>
       <c r="K15" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L15" s="25"/>
       <c r="M15" s="25"/>
@@ -4504,7 +4507,7 @@
         <v>151</v>
       </c>
       <c r="K16" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
@@ -4542,7 +4545,7 @@
         <v>151</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
@@ -4580,7 +4583,7 @@
         <v>151</v>
       </c>
       <c r="K18" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
@@ -4618,7 +4621,7 @@
         <v>151</v>
       </c>
       <c r="K19" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L19" s="25"/>
       <c r="M19" s="25"/>
@@ -4656,7 +4659,7 @@
         <v>151</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
@@ -4694,7 +4697,7 @@
         <v>151</v>
       </c>
       <c r="K21" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
@@ -4732,7 +4735,7 @@
         <v>151</v>
       </c>
       <c r="K22" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L22" s="25"/>
       <c r="M22" s="25"/>
@@ -4770,7 +4773,7 @@
         <v>151</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L23" s="25"/>
       <c r="M23" s="25"/>
@@ -4808,7 +4811,7 @@
         <v>151</v>
       </c>
       <c r="K24" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
@@ -4846,7 +4849,7 @@
         <v>151</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
@@ -4884,7 +4887,7 @@
         <v>151</v>
       </c>
       <c r="K26" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L26" s="25"/>
       <c r="M26" s="25"/>
@@ -4922,7 +4925,7 @@
         <v>151</v>
       </c>
       <c r="K27" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L27" s="25"/>
       <c r="M27" s="25"/>
@@ -4960,7 +4963,7 @@
         <v>151</v>
       </c>
       <c r="K28" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L28" s="25"/>
       <c r="M28" s="25"/>
@@ -4998,7 +5001,7 @@
         <v>151</v>
       </c>
       <c r="K29" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L29" s="25"/>
       <c r="M29" s="25"/>
@@ -5036,7 +5039,7 @@
         <v>151</v>
       </c>
       <c r="K30" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L30" s="25"/>
       <c r="M30" s="25"/>
@@ -5074,7 +5077,7 @@
         <v>151</v>
       </c>
       <c r="K31" s="25" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="L31" s="25"/>
       <c r="M31" s="25"/>
@@ -5148,17 +5151,17 @@
       <c r="E33" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="F33" s="31">
-        <v>45111</v>
+      <c r="F33" s="31" t="s">
+        <v>207</v>
       </c>
       <c r="G33" s="32" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
       <c r="H33" s="32" t="s">
-        <v>160</v>
+        <v>205</v>
       </c>
       <c r="I33" s="32" t="s">
-        <v>161</v>
+        <v>206</v>
       </c>
       <c r="J33" s="33" t="s">
         <v>110</v>
@@ -5192,17 +5195,17 @@
       <c r="E34" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="F34" s="31">
-        <v>45111</v>
+      <c r="F34" s="31" t="s">
+        <v>207</v>
       </c>
       <c r="G34" s="32" t="s">
-        <v>162</v>
+        <v>208</v>
       </c>
       <c r="H34" s="32" t="s">
-        <v>163</v>
+        <v>209</v>
       </c>
       <c r="I34" s="32" t="s">
-        <v>164</v>
+        <v>210</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>110</v>
@@ -5236,17 +5239,17 @@
       <c r="E35" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="F35" s="31">
-        <v>45111</v>
+      <c r="F35" s="31" t="s">
+        <v>207</v>
       </c>
       <c r="G35" s="32" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="H35" s="32" t="s">
-        <v>166</v>
+        <v>212</v>
       </c>
       <c r="I35" s="32" t="s">
-        <v>167</v>
+        <v>213</v>
       </c>
       <c r="J35" s="33" t="s">
         <v>110</v>
@@ -5280,17 +5283,17 @@
       <c r="E36" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="F36" s="31">
-        <v>45111</v>
+      <c r="F36" s="31" t="s">
+        <v>207</v>
       </c>
       <c r="G36" s="32" t="s">
-        <v>168</v>
+        <v>214</v>
       </c>
       <c r="H36" s="32" t="s">
-        <v>169</v>
+        <v>215</v>
       </c>
       <c r="I36" s="32" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="J36" s="33" t="s">
         <v>110</v>
@@ -5303,13 +5306,13 @@
         <v>110</v>
       </c>
       <c r="N36" s="33" t="s">
-        <v>209</v>
+        <v>178</v>
       </c>
       <c r="O36" s="33" t="s">
         <v>110</v>
       </c>
       <c r="P36" s="33" t="s">
-        <v>210</v>
+        <v>179</v>
       </c>
       <c r="Q36" s="25"/>
       <c r="R36" s="26"/>
@@ -5334,17 +5337,17 @@
       <c r="E37" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="F37" s="31">
-        <v>45111</v>
+      <c r="F37" s="31" t="s">
+        <v>207</v>
       </c>
       <c r="G37" s="32" t="s">
-        <v>171</v>
+        <v>216</v>
       </c>
       <c r="H37" s="32" t="s">
-        <v>172</v>
+        <v>217</v>
       </c>
       <c r="I37" s="32" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="J37" s="33" t="s">
         <v>110</v>
@@ -5357,13 +5360,13 @@
         <v>110</v>
       </c>
       <c r="N37" s="33" t="s">
-        <v>211</v>
+        <v>180</v>
       </c>
       <c r="O37" s="33" t="s">
         <v>110</v>
       </c>
       <c r="P37" s="33" t="s">
-        <v>210</v>
+        <v>179</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="26"/>
@@ -5403,13 +5406,13 @@
         <v>110</v>
       </c>
       <c r="N38" s="33" t="s">
-        <v>212</v>
+        <v>181</v>
       </c>
       <c r="O38" s="33" t="s">
         <v>110</v>
       </c>
       <c r="P38" s="33" t="s">
-        <v>213</v>
+        <v>182</v>
       </c>
       <c r="Q38" s="25"/>
       <c r="R38" s="26" t="s">
@@ -5440,13 +5443,13 @@
         <v>45111</v>
       </c>
       <c r="G39" s="32" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="H39" s="32" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="I39" s="32" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="J39" s="33" t="s">
         <v>110</v>
@@ -5459,13 +5462,13 @@
         <v>110</v>
       </c>
       <c r="N39" s="33" t="s">
-        <v>214</v>
+        <v>183</v>
       </c>
       <c r="O39" s="33" t="s">
         <v>151</v>
       </c>
       <c r="P39" s="33" t="s">
-        <v>215</v>
+        <v>184</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="26"/>
@@ -5494,13 +5497,13 @@
         <v>45111</v>
       </c>
       <c r="G40" s="32" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="H40" s="32" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="I40" s="32" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="J40" s="33" t="s">
         <v>110</v>
@@ -5513,13 +5516,13 @@
         <v>110</v>
       </c>
       <c r="N40" s="33" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
       <c r="O40" s="33" t="s">
         <v>151</v>
       </c>
       <c r="P40" s="33" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
       <c r="Q40" s="25"/>
       <c r="R40" s="26"/>
@@ -5548,13 +5551,13 @@
         <v>45111</v>
       </c>
       <c r="G41" s="32" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="H41" s="32" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="I41" s="32" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="J41" s="33" t="s">
         <v>110</v>
@@ -5567,13 +5570,13 @@
         <v>110</v>
       </c>
       <c r="N41" s="33" t="s">
-        <v>218</v>
+        <v>187</v>
       </c>
       <c r="O41" s="33" t="s">
         <v>151</v>
       </c>
       <c r="P41" s="33" t="s">
-        <v>215</v>
+        <v>184</v>
       </c>
       <c r="Q41" s="25"/>
       <c r="R41" s="26"/>
@@ -5602,13 +5605,13 @@
         <v>45111</v>
       </c>
       <c r="G42" s="32" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="H42" s="32" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="I42" s="32" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="J42" s="33" t="s">
         <v>110</v>
@@ -5621,13 +5624,13 @@
         <v>110</v>
       </c>
       <c r="N42" s="33" t="s">
-        <v>219</v>
+        <v>188</v>
       </c>
       <c r="O42" s="33" t="s">
         <v>151</v>
       </c>
       <c r="P42" s="33" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="Q42" s="25"/>
       <c r="R42" s="26"/>
@@ -5656,13 +5659,13 @@
         <v>45111</v>
       </c>
       <c r="G43" s="32" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="H43" s="32" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="I43" s="32" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="J43" s="33" t="s">
         <v>110</v>
@@ -5675,13 +5678,13 @@
         <v>110</v>
       </c>
       <c r="N43" s="33" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
       <c r="O43" s="33" t="s">
         <v>151</v>
       </c>
       <c r="P43" s="33" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="Q43" s="25"/>
       <c r="R43" s="26"/>
@@ -5710,13 +5713,13 @@
         <v>45111</v>
       </c>
       <c r="G44" s="32" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="H44" s="32" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="I44" s="32" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="J44" s="33" t="s">
         <v>110</v>
@@ -5729,13 +5732,13 @@
         <v>110</v>
       </c>
       <c r="N44" s="33" t="s">
-        <v>223</v>
+        <v>192</v>
       </c>
       <c r="O44" s="33" t="s">
         <v>151</v>
       </c>
       <c r="P44" s="33" t="s">
-        <v>224</v>
+        <v>193</v>
       </c>
       <c r="Q44" s="25"/>
       <c r="R44" s="26"/>
@@ -5760,17 +5763,17 @@
       <c r="E45" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="F45" s="31">
-        <v>45111</v>
+      <c r="F45" s="31" t="s">
+        <v>207</v>
       </c>
       <c r="G45" s="32" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="H45" s="32" t="s">
-        <v>192</v>
+        <v>219</v>
       </c>
       <c r="I45" s="32" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="J45" s="33" t="s">
         <v>110</v>
@@ -5783,13 +5786,13 @@
         <v>110</v>
       </c>
       <c r="N45" s="33" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="O45" s="33" t="s">
         <v>151</v>
       </c>
       <c r="P45" s="33" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="Q45" s="25"/>
       <c r="R45" s="26"/>
@@ -5814,17 +5817,17 @@
       <c r="E46" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="F46" s="31">
-        <v>45111</v>
+      <c r="F46" s="31" t="s">
+        <v>207</v>
       </c>
       <c r="G46" s="32" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="H46" s="32" t="s">
-        <v>195</v>
+        <v>222</v>
       </c>
       <c r="I46" s="32" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="J46" s="33" t="s">
         <v>110</v>
@@ -5837,13 +5840,13 @@
         <v>110</v>
       </c>
       <c r="N46" s="33" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="O46" s="33" t="s">
         <v>151</v>
       </c>
       <c r="P46" s="33" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="Q46" s="25"/>
       <c r="R46" s="26"/>
@@ -5868,17 +5871,17 @@
       <c r="E47" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="F47" s="31">
-        <v>45111</v>
+      <c r="F47" s="31" t="s">
+        <v>207</v>
       </c>
       <c r="G47" s="32" t="s">
-        <v>197</v>
+        <v>224</v>
       </c>
       <c r="H47" s="32" t="s">
-        <v>198</v>
+        <v>225</v>
       </c>
       <c r="I47" s="32" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
       <c r="J47" s="33" t="s">
         <v>110</v>
@@ -5891,13 +5894,13 @@
         <v>110</v>
       </c>
       <c r="N47" s="33" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="O47" s="33" t="s">
         <v>151</v>
       </c>
       <c r="P47" s="33" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>
@@ -5922,17 +5925,17 @@
       <c r="E48" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="F48" s="31">
-        <v>45111</v>
+      <c r="F48" s="31" t="s">
+        <v>207</v>
       </c>
       <c r="G48" s="32" t="s">
-        <v>200</v>
+        <v>227</v>
       </c>
       <c r="H48" s="32" t="s">
-        <v>201</v>
+        <v>228</v>
       </c>
       <c r="I48" s="32" t="s">
-        <v>202</v>
+        <v>229</v>
       </c>
       <c r="J48" s="33" t="s">
         <v>110</v>
@@ -5945,13 +5948,13 @@
         <v>110</v>
       </c>
       <c r="N48" s="33" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="O48" s="33" t="s">
         <v>151</v>
       </c>
       <c r="P48" s="33" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
       <c r="Q48" s="25"/>
       <c r="R48" s="26"/>
@@ -5976,17 +5979,17 @@
       <c r="E49" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="F49" s="31">
-        <v>45111</v>
+      <c r="F49" s="31" t="s">
+        <v>207</v>
       </c>
       <c r="G49" s="32" t="s">
-        <v>203</v>
+        <v>230</v>
       </c>
       <c r="H49" s="32" t="s">
-        <v>204</v>
+        <v>231</v>
       </c>
       <c r="I49" s="32" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
       <c r="J49" s="33" t="s">
         <v>110</v>
@@ -5999,13 +6002,13 @@
         <v>110</v>
       </c>
       <c r="N49" s="33" t="s">
-        <v>232</v>
+        <v>201</v>
       </c>
       <c r="O49" s="33" t="s">
         <v>110</v>
       </c>
       <c r="P49" s="33" t="s">
-        <v>210</v>
+        <v>179</v>
       </c>
       <c r="Q49" s="25"/>
       <c r="R49" s="26"/>
@@ -6030,17 +6033,17 @@
       <c r="E50" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="F50" s="31">
-        <v>45111</v>
+      <c r="F50" s="31" t="s">
+        <v>207</v>
       </c>
       <c r="G50" s="32" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
       <c r="H50" s="32" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
       <c r="I50" s="32" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="J50" s="33" t="s">
         <v>110</v>
@@ -6053,13 +6056,13 @@
         <v>110</v>
       </c>
       <c r="N50" s="33" t="s">
-        <v>233</v>
+        <v>202</v>
       </c>
       <c r="O50" s="33" t="s">
         <v>110</v>
       </c>
       <c r="P50" s="33" t="s">
-        <v>210</v>
+        <v>179</v>
       </c>
       <c r="Q50" s="25"/>
       <c r="R50" s="26"/>

</xml_diff>